<commit_message>
Problem beim Erstellen der Docker-Container mit skaffold gelöst
</commit_message>
<xml_diff>
--- a/Troubleshooting.xlsx
+++ b/Troubleshooting.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\3_Big_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\3_Big_Data\github\BigData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{A11B1F65-C420-46AB-B039-470F679251CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2554405-04B3-47AD-B9AD-5DDF1796C3CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21220"/>
+    <workbookView xWindow="-33017" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>Deployment and Development</t>
   </si>
@@ -121,12 +121,30 @@
   </si>
   <si>
     <t>use powershell commands</t>
+  </si>
+  <si>
+    <t>skaffold Docker container erstellen</t>
+  </si>
+  <si>
+    <t>/bin/sh: apt-get: not found</t>
+  </si>
+  <si>
+    <t>unable to stream build output: The command '/bin/sh -c apt-get update &amp;&amp; apt-get install -y python3 python3-pip' returned a non-zero code: 127. Please fix the Dockerfile and try again..</t>
+  </si>
+  <si>
+    <t xml:space="preserve">apt get not installes </t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/31876031/the-command-bin-sh-c-returned-a-non-zero-code-127</t>
+  </si>
+  <si>
+    <t>Links</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -490,27 +508,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:I15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B4:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="25.76171875" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="36.64453125" customWidth="1"/>
-    <col min="7" max="7" width="22.5859375" customWidth="1"/>
-    <col min="8" max="8" width="35.3515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.69140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.3828125" customWidth="1"/>
+    <col min="5" max="6" width="36.61328125" customWidth="1"/>
+    <col min="7" max="7" width="22.61328125" customWidth="1"/>
+    <col min="8" max="8" width="35.3828125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.5">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -535,8 +555,11 @@
       <c r="I8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="2:9" ht="57.35" x14ac:dyDescent="0.5">
+      <c r="J8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" ht="58.3" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
         <v>27</v>
       </c>
@@ -559,7 +582,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="86.7" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="2:10" ht="86.7" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B10" s="1" t="s">
         <v>0</v>
       </c>
@@ -581,7 +604,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="71.7" x14ac:dyDescent="0.5">
+    <row r="11" spans="2:10" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="B11" t="s">
         <v>14</v>
       </c>
@@ -598,7 +621,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="2:9" ht="100.35" x14ac:dyDescent="0.5">
+    <row r="12" spans="2:10" ht="102" x14ac:dyDescent="0.4">
       <c r="B12" t="s">
         <v>14</v>
       </c>
@@ -621,13 +644,26 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.5">
-      <c r="D13" s="6"/>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.5">
-      <c r="D14" s="6"/>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.5">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" ht="63" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="D14" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" t="s">
+        <v>32</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.4">
       <c r="D15" s="4"/>
     </row>
   </sheetData>

</xml_diff>